<commit_message>
add repro code to TOGS-lof6.xlsx to suppress copyrighted images.
</commit_message>
<xml_diff>
--- a/figureinfo/TOGS-lof6.xlsx
+++ b/figureinfo/TOGS-lof6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Rprojects\HistDataVis\figureinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB26E216-413E-4B09-A41A-E5017F24E9F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687975DF-2295-4F64-9E7B-D15F72D14E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="555" windowWidth="24285" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -598,9 +598,6 @@
     <t>06_14-galton-table-stigler1989.png</t>
   </si>
   <si>
-    <t>06_15a-galton-interp2.pdf, 06_15b-galton-interp3.pdf</t>
-  </si>
-  <si>
     <t>06_16-galton1886-corr.png</t>
   </si>
   <si>
@@ -1363,18 +1360,12 @@
     <t xml:space="preserve">Galton’s Table I on the relationship between heights of parents and their children. Entries in the table are the number of adult children. </t>
   </si>
   <si>
-    <t xml:space="preserve">Are construction of Galton’s method for finding contours of approximately equal frequency in the relation between heights of parents and their children. Left: The original data from his table (Figure 6.14) are shown in a small font (dark); the smoothed values are shown in a large font (light). Right: the lines joining the means of y|x and the means of x|y are added, together with the corresponding regression lines. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Galton’s smoothed correlation diagram for the data on heights of parents and children, showing one ellipse of constant frequency. The geometric relations between the regression lines and the tangent lines and major and minor axes are also shown. </t>
   </si>
   <si>
     <t xml:space="preserve">Russell’s plot of absolute magnitude against spectral class. </t>
   </si>
   <si>
-    <t xml:space="preserve">Hertzsprung–Russell diagrams for a collection of stars in the CYG OB1 star cluster. Left: regression line and data ellipse covering 50% of the points, fit using standard least-squares methods; right: regression line and 50% data ellipse using a robust method which is insensitive to the obvious unusual points in the upper left corner. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Phillips’s data on wage inflation and unemployment, 1861–1913, with the fitted Phillips curve. Points used in the fitting process are shown by + signs. </t>
   </si>
   <si>
@@ -1711,9 +1702,6 @@
     <t>A. W. Phillips, “The Relation between Unemployment and the Rate of Change of Money Wage Rates in the United Kingdom, 1861–1957,” Economica, 25:100 (1958), pp. 283–299, fig. 6.</t>
   </si>
   <si>
-    <t>Reformatted from Franz H. Messerli, “Chocolate Consumption, Cognitive Function, and Nobel Laureates,” The New Eng- land Journal of Medicine, 367:16 (2012), pp. 1562–1564, fig. 1. © 2012 Massachusetts Medical Society. Reprinted with permission from Massachusetts Medical Society.</t>
-  </si>
-  <si>
     <t>Reformatted from Michael Friendly, “The Golden Age of Statistical Graphics,” Statistical Science, 23:4 (2008), pp. 502–535, fig. 1.</t>
   </si>
   <si>
@@ -1898,6 +1886,18 @@
   </si>
   <si>
     <t>repro</t>
+  </si>
+  <si>
+    <t>06_15-galton-interp2.png, 06_15-galton-interp3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A reconstruction of Galton’s method for finding contours of approximately equal frequency in the relation between heights of parents and their children. Top: The original data from his table (Figure 6.14) are shown in a small font (dark); the smoothed values are shown in a large font (light). Bottom: the lines joining the means of y|x and the means of x|y are added, together with the corresponding regression lines. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hertzsprung–Russell diagrams for a collection of stars in the CYG OB1 star cluster. Top: regression line and data ellipse covering 50% of the points, fit using standard least-squares methods; bottom: regression line and 50% data ellipse using a robust method which is insensitive to the obvious unusual points in the upper left corner. </t>
+  </si>
+  <si>
+    <t>© The Authors. Redrawn from Franz H. Messerli, “Chocolate Consumption, Cognitive Function, and Nobel Laureates,” The New Eng- land Journal of Medicine, 367:16 (2012), pp. 1562–1564, fig. 1.</t>
   </si>
 </sst>
 </file>
@@ -2252,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2306,13 +2306,13 @@
         <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="G2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2332,13 +2332,13 @@
         <v>139</v>
       </c>
       <c r="F3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G3" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="H3" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2358,13 +2358,13 @@
         <v>140</v>
       </c>
       <c r="F4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H4" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,13 +2384,13 @@
         <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H5" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,13 +2410,13 @@
         <v>142</v>
       </c>
       <c r="F6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H6" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2436,13 +2436,13 @@
         <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H7" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2462,13 +2462,13 @@
         <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H8" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2488,13 +2488,13 @@
         <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H9" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2514,13 +2514,13 @@
         <v>146</v>
       </c>
       <c r="F10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2540,13 +2540,13 @@
         <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H11" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2566,13 +2566,13 @@
         <v>148</v>
       </c>
       <c r="F12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H12" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2592,13 +2592,13 @@
         <v>149</v>
       </c>
       <c r="F13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H13" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2618,13 +2618,13 @@
         <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H14" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2644,13 +2644,13 @@
         <v>151</v>
       </c>
       <c r="F15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H15" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2670,13 +2670,13 @@
         <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H16" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2696,13 +2696,13 @@
         <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G17" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H17" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2722,13 +2722,13 @@
         <v>154</v>
       </c>
       <c r="F18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H18" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2748,13 +2748,13 @@
         <v>155</v>
       </c>
       <c r="F19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G19" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H19" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2774,13 +2774,13 @@
         <v>156</v>
       </c>
       <c r="F20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H20" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2800,13 +2800,13 @@
         <v>157</v>
       </c>
       <c r="F21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G21" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H21" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2826,13 +2826,13 @@
         <v>158</v>
       </c>
       <c r="F22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G22" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H22" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2852,13 +2852,13 @@
         <v>159</v>
       </c>
       <c r="F23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H23" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2878,13 +2878,13 @@
         <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H24" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,13 +2904,13 @@
         <v>161</v>
       </c>
       <c r="F25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H25" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2930,13 +2930,13 @@
         <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G26" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H26" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2956,13 +2956,13 @@
         <v>163</v>
       </c>
       <c r="F27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G27" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H27" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2982,13 +2982,13 @@
         <v>164</v>
       </c>
       <c r="F28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H28" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3008,13 +3008,13 @@
         <v>165</v>
       </c>
       <c r="F29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H29" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3034,13 +3034,13 @@
         <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H30" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3060,13 +3060,13 @@
         <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G31" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H31" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3086,13 +3086,13 @@
         <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G32" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H32" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3112,13 +3112,13 @@
         <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G33" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H33" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G34" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H34" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3164,13 +3164,13 @@
         <v>171</v>
       </c>
       <c r="F35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H35" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3190,13 +3190,13 @@
         <v>172</v>
       </c>
       <c r="F36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G36" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H36" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3216,13 +3216,13 @@
         <v>173</v>
       </c>
       <c r="F37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G37" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H37" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,13 +3242,13 @@
         <v>174</v>
       </c>
       <c r="F38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G38" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H38" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3268,13 +3268,13 @@
         <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G39" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H39" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3294,13 +3294,13 @@
         <v>176</v>
       </c>
       <c r="F40" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H40" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3320,13 +3320,13 @@
         <v>177</v>
       </c>
       <c r="F41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G41" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H41" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3346,13 +3346,13 @@
         <v>178</v>
       </c>
       <c r="F42" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H42" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3372,13 +3372,13 @@
         <v>179</v>
       </c>
       <c r="F43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H43" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3398,13 +3398,13 @@
         <v>180</v>
       </c>
       <c r="F44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G44" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H44" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3424,13 +3424,13 @@
         <v>181</v>
       </c>
       <c r="F45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H45" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3450,13 +3450,13 @@
         <v>182</v>
       </c>
       <c r="F46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G46" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H46" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3476,13 +3476,13 @@
         <v>183</v>
       </c>
       <c r="F47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G47" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H47" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3502,13 +3502,13 @@
         <v>184</v>
       </c>
       <c r="F48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H48" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3528,13 +3528,13 @@
         <v>185</v>
       </c>
       <c r="F49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G49" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H49" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3554,13 +3554,13 @@
         <v>186</v>
       </c>
       <c r="F50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G50" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H50" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3580,13 +3580,13 @@
         <v>187</v>
       </c>
       <c r="F51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G51" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H51" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3606,13 +3606,13 @@
         <v>188</v>
       </c>
       <c r="F52" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G52" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H52" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3632,13 +3632,13 @@
         <v>189</v>
       </c>
       <c r="F53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G53" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H53" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3658,13 +3658,13 @@
         <v>190</v>
       </c>
       <c r="F54" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G54" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H54" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3684,13 +3684,13 @@
         <v>191</v>
       </c>
       <c r="F55" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G55" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H55" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3707,16 +3707,16 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>192</v>
+        <v>622</v>
       </c>
       <c r="F56" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G56" t="s">
-        <v>447</v>
+        <v>623</v>
       </c>
       <c r="H56" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3733,16 +3733,16 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G57" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H57" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3759,16 +3759,16 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G58" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H58" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3785,16 +3785,16 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F59" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G59" t="s">
-        <v>450</v>
+        <v>624</v>
       </c>
       <c r="H59" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3811,16 +3811,16 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F60" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G60" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H60" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3837,16 +3837,16 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F61" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G61" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H61" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3863,16 +3863,16 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F62" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G62" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H62" t="s">
-        <v>563</v>
+        <v>625</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3889,16 +3889,16 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F63" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G63" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H63" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3915,16 +3915,16 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F64" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G64" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H64" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3941,16 +3941,16 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F65" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G65" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H65" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3967,16 +3967,16 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F66" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G66" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="H66" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3993,16 +3993,16 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="F67" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G67" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H67" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4019,16 +4019,16 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F68" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G68" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H68" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4045,16 +4045,16 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G69" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="H69" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4071,16 +4071,16 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F70" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G70" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="H70" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4097,16 +4097,16 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G71" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H71" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4123,16 +4123,16 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F72" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G72" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H72" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4149,16 +4149,16 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F73" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G73" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H73" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4175,16 +4175,16 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F74" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G74" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H74" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,16 +4201,16 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F75" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G75" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="H75" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4227,16 +4227,16 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F76" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G76" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="H76" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4253,16 +4253,16 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F77" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G77" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="H77" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4279,16 +4279,16 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F78" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G78" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="H78" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4305,16 +4305,16 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F79" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G79" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H79" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4331,16 +4331,16 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F80" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G80" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="H80" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4357,16 +4357,16 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F81" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G81" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="H81" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4383,16 +4383,16 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F82" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G82" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="H82" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4409,16 +4409,16 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F83" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G83" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="H83" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4435,16 +4435,16 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F84" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G84" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H84" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4461,16 +4461,16 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G85" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H85" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4487,16 +4487,16 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F86" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G86" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H86" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4513,16 +4513,16 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F87" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G87" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H87" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4539,16 +4539,16 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F88" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G88" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H88" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4565,16 +4565,16 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F89" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G89" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="H89" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4591,16 +4591,16 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F90" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G90" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H90" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4617,16 +4617,16 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F91" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G91" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H91" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4643,16 +4643,16 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F92" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G92" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H92" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4669,16 +4669,16 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F93" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G93" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H93" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4695,16 +4695,16 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F94" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G94" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H94" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4721,16 +4721,16 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F95" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G95" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="H95" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4747,16 +4747,16 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F96" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G96" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="H96" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4773,16 +4773,16 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F97" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G97" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H97" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4799,16 +4799,16 @@
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="F98" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G98" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="H98" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4825,16 +4825,16 @@
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F99" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G99" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="H99" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4851,16 +4851,16 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F100" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G100" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H100" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4877,16 +4877,16 @@
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F101" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G101" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="H101" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4903,16 +4903,16 @@
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F102" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G102" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H102" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4929,16 +4929,16 @@
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F103" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G103" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H103" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4955,16 +4955,16 @@
         <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F104" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G104" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H104" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4981,16 +4981,16 @@
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F105" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G105" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H105" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5007,16 +5007,16 @@
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F106" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G106" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H106" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5033,16 +5033,16 @@
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F107" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G107" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H107" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5059,16 +5059,16 @@
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F108" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G108" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="H108" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5085,16 +5085,16 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F109" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G109" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="H109" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5111,16 +5111,16 @@
         <v>1</v>
       </c>
       <c r="E110" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F110" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G110" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="H110" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5137,16 +5137,16 @@
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F111" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G111" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H111" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,16 +5163,16 @@
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F112" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G112" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="H112" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5189,16 +5189,16 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F113" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G113" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="H113" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5215,16 +5215,16 @@
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F114" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G114" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="H114" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,16 +5241,16 @@
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F115" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G115" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H115" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5267,16 +5267,16 @@
         <v>1</v>
       </c>
       <c r="E116" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F116" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G116" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H116" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5293,16 +5293,16 @@
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F117" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G117" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H117" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5319,16 +5319,16 @@
         <v>1</v>
       </c>
       <c r="E118" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F118" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G118" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="H118" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5345,16 +5345,16 @@
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F119" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G119" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H119" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5371,16 +5371,16 @@
         <v>1</v>
       </c>
       <c r="E120" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F120" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G120" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="H120" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5397,16 +5397,16 @@
         <v>1</v>
       </c>
       <c r="E121" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F121" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G121" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H121" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5423,16 +5423,16 @@
         <v>1</v>
       </c>
       <c r="E122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F122" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G122" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H122" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5449,16 +5449,16 @@
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F123" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G123" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H123" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5475,16 +5475,16 @@
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F124" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G124" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H124" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5501,16 +5501,16 @@
         <v>1</v>
       </c>
       <c r="E125" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F125" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G125" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H125" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5527,16 +5527,16 @@
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F126" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G126" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H126" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5553,16 +5553,16 @@
         <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F127" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G127" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H127" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5579,16 +5579,16 @@
         <v>1</v>
       </c>
       <c r="E128" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F128" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G128" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H128" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5605,16 +5605,16 @@
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="F129" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G129" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H129" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5631,16 +5631,16 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F130" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G130" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="H130" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5657,16 +5657,16 @@
         <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F131" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G131" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="H131" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5683,16 +5683,16 @@
         <v>1</v>
       </c>
       <c r="E132" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F132" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G132" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H132" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some images in Ch 6
</commit_message>
<xml_diff>
--- a/figureinfo/TOGS-lof6.xlsx
+++ b/figureinfo/TOGS-lof6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Rprojects\HistDataVis\figureinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687975DF-2295-4F64-9E7B-D15F72D14E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60D8853-0132-402C-8F86-137F897A347C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,9 +559,6 @@
     <t>06_1-workers.png</t>
   </si>
   <si>
-    <t>06_2-halleygraph.png</t>
-  </si>
-  <si>
     <t>06_3-cotes1722-22.png</t>
   </si>
   <si>
@@ -607,12 +604,6 @@
     <t>06_18a-hertzsprung1.png, 06_18b-hertzsprung2.png</t>
   </si>
   <si>
-    <t>06_19-phillips-fig1-300dpi.png</t>
-  </si>
-  <si>
-    <t>06_20-phillips-fig6-300dpi.png</t>
-  </si>
-  <si>
     <t>06_21-nobel-chocolate.png</t>
   </si>
   <si>
@@ -1898,6 +1889,15 @@
   </si>
   <si>
     <t>© The Authors. Redrawn from Franz H. Messerli, “Chocolate Consumption, Cognitive Function, and Nobel Laureates,” The New Eng- land Journal of Medicine, 367:16 (2012), pp. 1562–1564, fig. 1.</t>
+  </si>
+  <si>
+    <t>06_2-halleygraph2.png</t>
+  </si>
+  <si>
+    <t>06_19-phillips-fig1-copyr.png</t>
+  </si>
+  <si>
+    <t>06_20-phillips-fig6-copyr.png</t>
   </si>
 </sst>
 </file>
@@ -2252,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2306,13 +2306,13 @@
         <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="G2" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2332,13 +2332,13 @@
         <v>139</v>
       </c>
       <c r="F3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G3" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="H3" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2358,13 +2358,13 @@
         <v>140</v>
       </c>
       <c r="F4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="H4" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,13 +2384,13 @@
         <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H5" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,13 +2410,13 @@
         <v>142</v>
       </c>
       <c r="F6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H6" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2436,13 +2436,13 @@
         <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G7" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="H7" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2462,13 +2462,13 @@
         <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G8" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H8" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2488,13 +2488,13 @@
         <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G9" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="H9" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2514,13 +2514,13 @@
         <v>146</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G10" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="H10" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2540,13 +2540,13 @@
         <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="H11" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2566,13 +2566,13 @@
         <v>148</v>
       </c>
       <c r="F12" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G12" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="H12" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2592,13 +2592,13 @@
         <v>149</v>
       </c>
       <c r="F13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G13" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H13" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2618,13 +2618,13 @@
         <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G14" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="H14" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2644,13 +2644,13 @@
         <v>151</v>
       </c>
       <c r="F15" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G15" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H15" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2670,13 +2670,13 @@
         <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G16" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H16" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2696,13 +2696,13 @@
         <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G17" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H17" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2722,13 +2722,13 @@
         <v>154</v>
       </c>
       <c r="F18" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G18" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H18" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2748,13 +2748,13 @@
         <v>155</v>
       </c>
       <c r="F19" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H19" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2774,13 +2774,13 @@
         <v>156</v>
       </c>
       <c r="F20" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G20" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="H20" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2800,13 +2800,13 @@
         <v>157</v>
       </c>
       <c r="F21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G21" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="H21" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2826,13 +2826,13 @@
         <v>158</v>
       </c>
       <c r="F22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G22" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H22" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2852,13 +2852,13 @@
         <v>159</v>
       </c>
       <c r="F23" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G23" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H23" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2878,13 +2878,13 @@
         <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G24" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="H24" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,13 +2904,13 @@
         <v>161</v>
       </c>
       <c r="F25" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G25" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="H25" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2930,13 +2930,13 @@
         <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G26" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H26" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2956,13 +2956,13 @@
         <v>163</v>
       </c>
       <c r="F27" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="G27" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H27" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2982,13 +2982,13 @@
         <v>164</v>
       </c>
       <c r="F28" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G28" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="H28" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3008,13 +3008,13 @@
         <v>165</v>
       </c>
       <c r="F29" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G29" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H29" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3034,13 +3034,13 @@
         <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G30" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="H30" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3060,13 +3060,13 @@
         <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="G31" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="H31" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3086,13 +3086,13 @@
         <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G32" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="H32" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3112,13 +3112,13 @@
         <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="G33" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H33" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G34" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H34" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3164,13 +3164,13 @@
         <v>171</v>
       </c>
       <c r="F35" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G35" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="H35" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3190,13 +3190,13 @@
         <v>172</v>
       </c>
       <c r="F36" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G36" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H36" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3216,13 +3216,13 @@
         <v>173</v>
       </c>
       <c r="F37" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G37" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="H37" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,13 +3242,13 @@
         <v>174</v>
       </c>
       <c r="F38" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G38" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="H38" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3268,13 +3268,13 @@
         <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G39" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H39" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3294,13 +3294,13 @@
         <v>176</v>
       </c>
       <c r="F40" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G40" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="H40" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3320,13 +3320,13 @@
         <v>177</v>
       </c>
       <c r="F41" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G41" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H41" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3346,13 +3346,13 @@
         <v>178</v>
       </c>
       <c r="F42" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G42" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H42" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3369,16 +3369,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>179</v>
+        <v>623</v>
       </c>
       <c r="F43" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G43" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H43" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3395,16 +3395,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F44" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G44" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H44" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3421,16 +3421,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F45" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G45" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H45" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3447,16 +3447,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F46" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G46" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H46" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3473,16 +3473,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F47" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G47" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H47" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3499,16 +3499,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F48" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G48" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H48" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3525,16 +3525,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F49" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G49" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H49" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3551,16 +3551,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F50" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G50" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="H50" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3577,16 +3577,16 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F51" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G51" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H51" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3603,16 +3603,16 @@
         <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F52" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G52" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H52" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3629,16 +3629,16 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F53" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G53" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="H53" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3655,16 +3655,16 @@
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F54" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G54" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H54" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3681,16 +3681,16 @@
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F55" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G55" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H55" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3707,16 +3707,16 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="F56" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G56" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="H56" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3733,16 +3733,16 @@
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F57" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G57" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H57" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3759,16 +3759,16 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F58" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G58" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H58" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3785,16 +3785,16 @@
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F59" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G59" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="H59" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3808,19 +3808,19 @@
         <v>65</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>195</v>
+        <v>624</v>
       </c>
       <c r="F60" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G60" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H60" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3834,19 +3834,19 @@
         <v>66</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>196</v>
+        <v>625</v>
       </c>
       <c r="F61" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G61" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H61" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3863,16 +3863,16 @@
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F62" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G62" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H62" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3889,16 +3889,16 @@
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F63" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G63" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H63" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3915,16 +3915,16 @@
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F64" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G64" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H64" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3941,16 +3941,16 @@
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F65" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G65" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H65" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3967,16 +3967,16 @@
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F66" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G66" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="H66" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3993,16 +3993,16 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="F67" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G67" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H67" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4019,16 +4019,16 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F68" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G68" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H68" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4045,16 +4045,16 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G69" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="H69" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4071,16 +4071,16 @@
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F70" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G70" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H70" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4097,16 +4097,16 @@
         <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F71" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G71" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H71" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4123,16 +4123,16 @@
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F72" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G72" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="H72" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4149,16 +4149,16 @@
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F73" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G73" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="H73" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4175,16 +4175,16 @@
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F74" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G74" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H74" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,16 +4201,16 @@
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F75" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G75" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H75" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4227,16 +4227,16 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F76" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G76" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="H76" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4253,16 +4253,16 @@
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F77" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G77" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H77" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4279,16 +4279,16 @@
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F78" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G78" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="H78" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4305,16 +4305,16 @@
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F79" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G79" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="H79" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4331,16 +4331,16 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F80" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G80" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="H80" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4357,16 +4357,16 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F81" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G81" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="H81" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4383,16 +4383,16 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F82" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G82" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="H82" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4409,16 +4409,16 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F83" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G83" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="H83" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4435,16 +4435,16 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F84" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G84" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="H84" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4461,16 +4461,16 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F85" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G85" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="H85" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4487,16 +4487,16 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F86" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G86" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="H86" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4513,16 +4513,16 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F87" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G87" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="H87" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4539,16 +4539,16 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F88" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G88" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H88" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4565,16 +4565,16 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F89" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G89" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="H89" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4591,16 +4591,16 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F90" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G90" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="H90" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4617,16 +4617,16 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F91" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G91" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="H91" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4643,16 +4643,16 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F92" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G92" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="H92" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4669,16 +4669,16 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F93" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G93" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="H93" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4695,16 +4695,16 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F94" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G94" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H94" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4721,16 +4721,16 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F95" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G95" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="H95" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4747,16 +4747,16 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F96" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G96" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H96" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4773,16 +4773,16 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F97" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G97" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H97" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4799,16 +4799,16 @@
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="F98" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G98" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="H98" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4825,16 +4825,16 @@
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F99" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G99" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="H99" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4851,16 +4851,16 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F100" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G100" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="H100" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4877,16 +4877,16 @@
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F101" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G101" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="H101" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4903,16 +4903,16 @@
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F102" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G102" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="H102" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4929,16 +4929,16 @@
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F103" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G103" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="H103" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4955,16 +4955,16 @@
         <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F104" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G104" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="H104" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4981,16 +4981,16 @@
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F105" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G105" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H105" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5007,16 +5007,16 @@
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F106" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G106" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H106" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5033,16 +5033,16 @@
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F107" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G107" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H107" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5059,16 +5059,16 @@
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F108" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G108" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="H108" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5085,16 +5085,16 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F109" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G109" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="H109" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5111,16 +5111,16 @@
         <v>1</v>
       </c>
       <c r="E110" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F110" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G110" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="H110" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5137,16 +5137,16 @@
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F111" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G111" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="H111" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,16 +5163,16 @@
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F112" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G112" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="H112" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5189,16 +5189,16 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F113" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G113" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="H113" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5215,16 +5215,16 @@
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F114" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G114" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="H114" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,16 +5241,16 @@
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F115" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G115" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="H115" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5267,16 +5267,16 @@
         <v>1</v>
       </c>
       <c r="E116" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F116" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G116" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="H116" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5293,16 +5293,16 @@
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F117" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G117" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="H117" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5319,16 +5319,16 @@
         <v>1</v>
       </c>
       <c r="E118" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F118" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G118" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="H118" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5345,16 +5345,16 @@
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F119" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G119" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="H119" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5371,16 +5371,16 @@
         <v>1</v>
       </c>
       <c r="E120" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F120" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G120" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H120" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5397,16 +5397,16 @@
         <v>1</v>
       </c>
       <c r="E121" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F121" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G121" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="H121" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5423,16 +5423,16 @@
         <v>1</v>
       </c>
       <c r="E122" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F122" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G122" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="H122" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5449,16 +5449,16 @@
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F123" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G123" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="H123" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5475,16 +5475,16 @@
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F124" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G124" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="H124" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5501,16 +5501,16 @@
         <v>1</v>
       </c>
       <c r="E125" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F125" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G125" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="H125" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5527,16 +5527,16 @@
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F126" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G126" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="H126" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5553,16 +5553,16 @@
         <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F127" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G127" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="H127" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5579,16 +5579,16 @@
         <v>1</v>
       </c>
       <c r="E128" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F128" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G128" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H128" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5605,16 +5605,16 @@
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F129" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G129" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H129" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5631,16 +5631,16 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F130" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G130" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="H130" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5657,16 +5657,16 @@
         <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F131" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G131" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="H131" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5683,16 +5683,16 @@
         <v>1</v>
       </c>
       <c r="E132" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F132" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G132" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="H132" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up .tif figs, delete not-used
</commit_message>
<xml_diff>
--- a/figureinfo/TOGS-lof6.xlsx
+++ b/figureinfo/TOGS-lof6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Rprojects\HistDataVis\figureinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60D8853-0132-402C-8F86-137F897A347C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF467D0-BF8C-4966-9347-1B61B28EE790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,9 +655,6 @@
     <t>08_3-halley-Lori-imago-detail.jpg</t>
   </si>
   <si>
-    <t>08_4-Lalanne_APC-1846-1.tif</t>
-  </si>
-  <si>
     <t>08_5-vauthier2.jpg</t>
   </si>
   <si>
@@ -790,9 +787,6 @@
     <t>P_13a-galton-summary-symbols.jpg, P_13b-galton1861-dec5-detail.png</t>
   </si>
   <si>
-    <t>P_14a-1870_race_mosaic.tif</t>
-  </si>
-  <si>
     <t>P_15-galton1881-isochronic-map.jpg</t>
   </si>
   <si>
@@ -1898,6 +1892,12 @@
   </si>
   <si>
     <t>06_20-phillips-fig6-copyr.png</t>
+  </si>
+  <si>
+    <t>08_14-Lalanne-fg14b.jpg</t>
+  </si>
+  <si>
+    <t>P_14-1870_race_mosaic-anno.jpg</t>
   </si>
 </sst>
 </file>
@@ -2252,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2274,7 +2274,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2306,13 +2306,13 @@
         <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="G2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2332,13 +2332,13 @@
         <v>139</v>
       </c>
       <c r="F3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G3" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="H3" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2358,13 +2358,13 @@
         <v>140</v>
       </c>
       <c r="F4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H4" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2384,13 +2384,13 @@
         <v>141</v>
       </c>
       <c r="F5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H5" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,13 +2410,13 @@
         <v>142</v>
       </c>
       <c r="F6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H6" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2436,13 +2436,13 @@
         <v>143</v>
       </c>
       <c r="F7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2462,13 +2462,13 @@
         <v>144</v>
       </c>
       <c r="F8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2488,13 +2488,13 @@
         <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H9" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2514,13 +2514,13 @@
         <v>146</v>
       </c>
       <c r="F10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H10" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2540,13 +2540,13 @@
         <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H11" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2566,13 +2566,13 @@
         <v>148</v>
       </c>
       <c r="F12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H12" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2592,13 +2592,13 @@
         <v>149</v>
       </c>
       <c r="F13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H13" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2618,13 +2618,13 @@
         <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H14" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2644,13 +2644,13 @@
         <v>151</v>
       </c>
       <c r="F15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G15" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2670,13 +2670,13 @@
         <v>152</v>
       </c>
       <c r="F16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G16" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H16" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2696,13 +2696,13 @@
         <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G17" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H17" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -2722,13 +2722,13 @@
         <v>154</v>
       </c>
       <c r="F18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G18" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H18" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2748,13 +2748,13 @@
         <v>155</v>
       </c>
       <c r="F19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H19" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2774,13 +2774,13 @@
         <v>156</v>
       </c>
       <c r="F20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G20" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H20" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2800,13 +2800,13 @@
         <v>157</v>
       </c>
       <c r="F21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H21" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2826,13 +2826,13 @@
         <v>158</v>
       </c>
       <c r="F22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G22" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H22" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2852,13 +2852,13 @@
         <v>159</v>
       </c>
       <c r="F23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G23" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H23" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2878,13 +2878,13 @@
         <v>160</v>
       </c>
       <c r="F24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G24" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2904,13 +2904,13 @@
         <v>161</v>
       </c>
       <c r="F25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G25" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H25" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2930,13 +2930,13 @@
         <v>162</v>
       </c>
       <c r="F26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G26" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H26" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2956,13 +2956,13 @@
         <v>163</v>
       </c>
       <c r="F27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G27" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2982,13 +2982,13 @@
         <v>164</v>
       </c>
       <c r="F28" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G28" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H28" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3008,13 +3008,13 @@
         <v>165</v>
       </c>
       <c r="F29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G29" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H29" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3034,13 +3034,13 @@
         <v>166</v>
       </c>
       <c r="F30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G30" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H30" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3060,13 +3060,13 @@
         <v>167</v>
       </c>
       <c r="F31" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G31" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H31" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3086,13 +3086,13 @@
         <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G32" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H32" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3112,13 +3112,13 @@
         <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G33" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H33" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>170</v>
       </c>
       <c r="F34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G34" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H34" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3164,13 +3164,13 @@
         <v>171</v>
       </c>
       <c r="F35" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G35" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H35" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -3190,13 +3190,13 @@
         <v>172</v>
       </c>
       <c r="F36" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G36" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H36" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -3216,13 +3216,13 @@
         <v>173</v>
       </c>
       <c r="F37" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G37" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H37" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3242,13 +3242,13 @@
         <v>174</v>
       </c>
       <c r="F38" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G38" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H38" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -3268,13 +3268,13 @@
         <v>175</v>
       </c>
       <c r="F39" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G39" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H39" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -3294,13 +3294,13 @@
         <v>176</v>
       </c>
       <c r="F40" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G40" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H40" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -3320,13 +3320,13 @@
         <v>177</v>
       </c>
       <c r="F41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G41" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H41" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3346,13 +3346,13 @@
         <v>178</v>
       </c>
       <c r="F42" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G42" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H42" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -3369,16 +3369,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F43" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G43" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H43" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -3398,13 +3398,13 @@
         <v>179</v>
       </c>
       <c r="F44" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G44" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H44" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3424,13 +3424,13 @@
         <v>180</v>
       </c>
       <c r="F45" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G45" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H45" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -3450,13 +3450,13 @@
         <v>181</v>
       </c>
       <c r="F46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G46" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H46" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3476,13 +3476,13 @@
         <v>182</v>
       </c>
       <c r="F47" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G47" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H47" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3502,13 +3502,13 @@
         <v>183</v>
       </c>
       <c r="F48" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G48" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H48" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -3528,13 +3528,13 @@
         <v>184</v>
       </c>
       <c r="F49" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G49" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H49" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -3554,13 +3554,13 @@
         <v>185</v>
       </c>
       <c r="F50" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G50" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H50" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -3580,13 +3580,13 @@
         <v>186</v>
       </c>
       <c r="F51" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G51" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H51" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -3606,13 +3606,13 @@
         <v>187</v>
       </c>
       <c r="F52" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G52" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H52" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -3632,13 +3632,13 @@
         <v>188</v>
       </c>
       <c r="F53" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="G53" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H53" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -3658,13 +3658,13 @@
         <v>189</v>
       </c>
       <c r="F54" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G54" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H54" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -3684,13 +3684,13 @@
         <v>190</v>
       </c>
       <c r="F55" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H55" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -3707,16 +3707,16 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F56" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G56" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="H56" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -3736,13 +3736,13 @@
         <v>191</v>
       </c>
       <c r="F57" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G57" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H57" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -3762,13 +3762,13 @@
         <v>192</v>
       </c>
       <c r="F58" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G58" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H58" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3788,13 +3788,13 @@
         <v>193</v>
       </c>
       <c r="F59" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G59" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H59" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -3811,16 +3811,16 @@
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F60" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G60" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H60" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -3837,16 +3837,16 @@
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F61" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G61" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H61" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3866,13 +3866,13 @@
         <v>194</v>
       </c>
       <c r="F62" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G62" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H62" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -3892,13 +3892,13 @@
         <v>195</v>
       </c>
       <c r="F63" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G63" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H63" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -3918,13 +3918,13 @@
         <v>196</v>
       </c>
       <c r="F64" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G64" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H64" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -3944,13 +3944,13 @@
         <v>197</v>
       </c>
       <c r="F65" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G65" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H65" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -3970,13 +3970,13 @@
         <v>198</v>
       </c>
       <c r="F66" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G66" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H66" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -3993,16 +3993,16 @@
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F67" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G67" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H67" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -4022,13 +4022,13 @@
         <v>199</v>
       </c>
       <c r="F68" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G68" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H68" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -4048,13 +4048,13 @@
         <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G69" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H69" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4074,13 +4074,13 @@
         <v>201</v>
       </c>
       <c r="F70" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G70" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H70" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4100,13 +4100,13 @@
         <v>202</v>
       </c>
       <c r="F71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G71" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H71" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4126,13 +4126,13 @@
         <v>203</v>
       </c>
       <c r="F72" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G72" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H72" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4152,13 +4152,13 @@
         <v>204</v>
       </c>
       <c r="F73" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G73" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H73" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4178,13 +4178,13 @@
         <v>205</v>
       </c>
       <c r="F74" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G74" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H74" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4204,13 +4204,13 @@
         <v>206</v>
       </c>
       <c r="F75" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G75" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H75" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4230,13 +4230,13 @@
         <v>207</v>
       </c>
       <c r="F76" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G76" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H76" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4256,13 +4256,13 @@
         <v>208</v>
       </c>
       <c r="F77" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G77" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H77" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4282,13 +4282,13 @@
         <v>209</v>
       </c>
       <c r="F78" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G78" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H78" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -4308,13 +4308,13 @@
         <v>210</v>
       </c>
       <c r="F79" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G79" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="H79" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -4331,16 +4331,16 @@
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>211</v>
+        <v>624</v>
       </c>
       <c r="F80" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G80" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H80" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -4357,16 +4357,16 @@
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F81" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G81" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H81" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -4383,16 +4383,16 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F82" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G82" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H82" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -4409,16 +4409,16 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F83" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G83" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H83" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -4435,16 +4435,16 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F84" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G84" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H84" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -4461,16 +4461,16 @@
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F85" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G85" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H85" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -4487,16 +4487,16 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F86" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G86" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H86" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -4513,16 +4513,16 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F87" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G87" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H87" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -4539,16 +4539,16 @@
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F88" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G88" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H88" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -4565,16 +4565,16 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F89" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G89" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H89" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -4591,16 +4591,16 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F90" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G90" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H90" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -4617,16 +4617,16 @@
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F91" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G91" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H91" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4643,16 +4643,16 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F92" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G92" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H92" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4669,16 +4669,16 @@
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F93" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G93" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H93" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4695,16 +4695,16 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F94" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G94" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H94" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -4721,16 +4721,16 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F95" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G95" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H95" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -4747,16 +4747,16 @@
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F96" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G96" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H96" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -4773,16 +4773,16 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F97" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G97" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H97" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4799,16 +4799,16 @@
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F98" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G98" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H98" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4825,16 +4825,16 @@
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F99" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G99" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H99" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -4851,16 +4851,16 @@
         <v>1</v>
       </c>
       <c r="E100" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F100" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G100" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="H100" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -4877,16 +4877,16 @@
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F101" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G101" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H101" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -4903,16 +4903,16 @@
         <v>1</v>
       </c>
       <c r="E102" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F102" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G102" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H102" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -4929,16 +4929,16 @@
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F103" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G103" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H103" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -4955,16 +4955,16 @@
         <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F104" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G104" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="H104" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -4981,16 +4981,16 @@
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F105" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G105" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="H105" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -5007,16 +5007,16 @@
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F106" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G106" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H106" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -5033,16 +5033,16 @@
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F107" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G107" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H107" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -5059,16 +5059,16 @@
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F108" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G108" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H108" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -5085,16 +5085,16 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F109" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G109" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H109" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -5111,16 +5111,16 @@
         <v>1</v>
       </c>
       <c r="E110" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F110" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G110" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H110" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -5137,16 +5137,16 @@
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F111" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="G111" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H111" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,16 +5163,16 @@
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F112" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G112" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H112" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -5189,16 +5189,16 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F113" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G113" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H113" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -5215,16 +5215,16 @@
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F114" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G114" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="H114" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,16 +5241,16 @@
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F115" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G115" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="H115" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -5267,16 +5267,16 @@
         <v>1</v>
       </c>
       <c r="E116" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F116" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G116" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H116" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -5293,16 +5293,16 @@
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F117" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G117" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="H117" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -5319,16 +5319,16 @@
         <v>1</v>
       </c>
       <c r="E118" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F118" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G118" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="H118" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -5345,16 +5345,16 @@
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F119" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G119" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="H119" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -5371,16 +5371,16 @@
         <v>1</v>
       </c>
       <c r="E120" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F120" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G120" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="H120" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -5397,16 +5397,16 @@
         <v>1</v>
       </c>
       <c r="E121" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F121" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G121" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H121" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -5423,16 +5423,16 @@
         <v>1</v>
       </c>
       <c r="E122" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F122" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="G122" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H122" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -5449,16 +5449,16 @@
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F123" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G123" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H123" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -5475,16 +5475,16 @@
         <v>1</v>
       </c>
       <c r="E124" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F124" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G124" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="H124" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -5501,16 +5501,16 @@
         <v>1</v>
       </c>
       <c r="E125" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F125" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="G125" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="H125" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -5527,16 +5527,16 @@
         <v>1</v>
       </c>
       <c r="E126" t="s">
-        <v>256</v>
+        <v>625</v>
       </c>
       <c r="F126" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G126" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="H126" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -5553,16 +5553,16 @@
         <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F127" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G127" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="H127" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -5579,16 +5579,16 @@
         <v>1</v>
       </c>
       <c r="E128" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F128" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G128" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="H128" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -5605,16 +5605,16 @@
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F129" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G129" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H129" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -5631,16 +5631,16 @@
         <v>1</v>
       </c>
       <c r="E130" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F130" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G130" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="H130" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -5657,16 +5657,16 @@
         <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F131" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G131" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H131" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -5683,16 +5683,16 @@
         <v>1</v>
       </c>
       <c r="E132" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F132" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G132" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="H132" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
   </sheetData>

</xml_diff>